<commit_message>
interview Info - 2
</commit_message>
<xml_diff>
--- a/Interview/companyAndInterviews.xlsx
+++ b/Interview/companyAndInterviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D_Work\Front-End\JavaScriptNotes\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC071BC-C1A8-4FE2-A6E8-4C97BDE9A5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C095AB01-21CB-4DF2-81A7-FEE6E6B23DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5303" yWindow="6157" windowWidth="21599" windowHeight="11423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5303" yWindow="4178" windowWidth="21599" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,11 +118,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>first/待定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>陌陌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>first/时间待定</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -552,15 +552,15 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
interview summary - 3
</commit_message>
<xml_diff>
--- a/Interview/companyAndInterviews.xlsx
+++ b/Interview/companyAndInterviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D_Work\Front-End\JavaScriptNotes\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C095AB01-21CB-4DF2-81A7-FEE6E6B23DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97C7478-DD0A-4ED6-AFBD-20FBC624A685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5303" yWindow="4178" windowWidth="21599" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="727" yWindow="6067" windowWidth="21600" windowHeight="11423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>company</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,14 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>first/22.01.19/电话/待定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>时间待定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>小黑盒</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -102,10 +94,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>first/22.01.20/视频/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>传智教育</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,7 +110,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>first/时间待定</t>
+    <t>first/22.01.19/电话/未通过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>first/22.01.20/视频/未通过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>first/22.01.24/视频/19:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>first/22.01.25/视频/18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>second/22.01.25/视频/12:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -457,8 +461,8 @@
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20.46484375" customWidth="1"/>
-    <col min="2" max="2" width="23.1328125" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" customWidth="1"/>
+    <col min="3" max="3" width="24.9296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
@@ -480,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -488,68 +492,68 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
@@ -557,10 +561,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>